<commit_message>
update lambda and delegate
</commit_message>
<xml_diff>
--- a/Git Project Management Tool/git.xlsx
+++ b/Git Project Management Tool/git.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jansson\Desktop\Full-stack\Git Project Management Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janss\Desktop\Full-stack\Git Project Management Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F83471-B8E9-408B-BDB1-521839822C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF4805-9D60-40A9-82C7-159AC0DB6E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="-14835" windowWidth="27000" windowHeight="13335" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="导航栏" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="从工作区到本地仓库" sheetId="5" r:id="rId3"/>
     <sheet name="Linux常见命令" sheetId="2" r:id="rId4"/>
     <sheet name="员工使用场景" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
-    <sheet name="负责人使用场景" sheetId="6" r:id="rId7"/>
+    <sheet name="负责人使用场景" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -556,9 +556,6 @@
     <t>（可忽略）查看当前 Git 仓库中已配置的远程仓库</t>
   </si>
   <si>
-    <t>4. 推送到Github</t>
-  </si>
-  <si>
     <t>1. 配置SSH公钥</t>
   </si>
   <si>
@@ -734,6 +731,9 @@
   </si>
   <si>
     <t>获得批准后，合并到主分支</t>
+  </si>
+  <si>
+    <t>4. 推送到Github(先git pull origin main)</t>
   </si>
 </sst>
 </file>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3879,13 +3879,13 @@
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="18:27" x14ac:dyDescent="0.25">
       <c r="R68" s="1"/>
       <c r="S68" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -3894,15 +3894,15 @@
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
       <c r="Z68" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA68" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="18:27" x14ac:dyDescent="0.25">
       <c r="R69" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S69" s="15"/>
       <c r="T69" s="15"/>
@@ -3912,10 +3912,10 @@
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
       <c r="Z69" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA69" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="18:27" x14ac:dyDescent="0.25">
@@ -3925,12 +3925,12 @@
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
       <c r="W70" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
       <c r="Z70" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="18:27" x14ac:dyDescent="0.25">
@@ -3954,7 +3954,7 @@
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
       <c r="Z72" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="18:27" x14ac:dyDescent="0.25">
@@ -3969,10 +3969,10 @@
       <c r="X73" s="1"/>
       <c r="Y73" s="1"/>
       <c r="Z73" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AA73" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3993,8 +3993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17947A92-9EE2-41F6-B11F-1071544CFE37}">
   <dimension ref="C2:P127"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:W9"/>
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4204,7 +4204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97D57A9-6E18-41B3-80BA-097061AF2973}">
   <dimension ref="C2:K100"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -4384,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC8E6EB-D299-468C-92E1-93201DF9EC15}">
   <dimension ref="E2:W109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L106" sqref="L106"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4395,7 +4395,7 @@
   <sheetData>
     <row r="2" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E2" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -5613,42 +5613,42 @@
     </row>
     <row r="59" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E59" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="5:23" x14ac:dyDescent="0.25">
       <c r="F61" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="5:23" x14ac:dyDescent="0.25">
       <c r="F63" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F67" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F73" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="5:6" x14ac:dyDescent="0.25">
@@ -5674,57 +5674,57 @@
     </row>
     <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F93" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F95" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5734,6 +5734,223 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615230FB-16C8-4EA2-80EF-B5114F8D97AE}">
+  <dimension ref="E4:L129"/>
+  <sheetViews>
+    <sheetView topLeftCell="C112" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G24" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G28" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F30" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H38" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="G67" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E79" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F81" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G83" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F85" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G87" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G88" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F90" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G92" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F95" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="G97" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H99" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H100" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="109" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F109" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="G111" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I111" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="113" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F113" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="115" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H115" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F121" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="123" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G123" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="125" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H125" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J125" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G127" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="129" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H129" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K129" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CF1F86-48CF-417B-90E9-D9D2DB833408}">
   <dimension ref="C2:H28"/>
   <sheetViews>
@@ -5745,7 +5962,7 @@
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -5755,7 +5972,7 @@
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5765,7 +5982,7 @@
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -5775,7 +5992,7 @@
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -5785,7 +6002,7 @@
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -5795,7 +6012,7 @@
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -5805,7 +6022,7 @@
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -5815,7 +6032,7 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -5825,7 +6042,7 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -5835,7 +6052,7 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -5845,7 +6062,7 @@
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -5855,7 +6072,7 @@
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -5865,7 +6082,7 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5875,7 +6092,7 @@
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -5885,7 +6102,7 @@
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -5895,7 +6112,7 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -5905,7 +6122,7 @@
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5915,7 +6132,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5925,7 +6142,7 @@
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -5935,7 +6152,7 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -5945,7 +6162,7 @@
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -5955,7 +6172,7 @@
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -5965,7 +6182,7 @@
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -5975,7 +6192,7 @@
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -5985,7 +6202,7 @@
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -5995,7 +6212,7 @@
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -6005,7 +6222,7 @@
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -6016,221 +6233,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615230FB-16C8-4EA2-80EF-B5114F8D97AE}">
-  <dimension ref="E4:L129"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E21" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G24" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G26" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="L27" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G28" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H34" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G36" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H38" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="G67" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="H69" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E79" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F81" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G83" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F85" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G87" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H87" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G88" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F90" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G92" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F95" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="97" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="G97" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="99" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H99" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="100" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H100" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="109" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F109" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="111" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="G111" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I111" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="113" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F113" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="115" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="H115" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="121" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F121" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="123" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="G123" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="125" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="H125" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="J125" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="127" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="G127" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="129" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H129" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="K129" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>